<commit_message>
Changed perspective to overhead.  Main menu is toggleable
</commit_message>
<xml_diff>
--- a/Game development tracking sheet.xlsx
+++ b/Game development tracking sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul\Documents\S3\asdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{548D2588-A3BD-4428-9025-838D7BE23358}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D23DA3EA-25DE-4383-89FA-8CCE2C020B9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +546,7 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">

</xml_diff>

<commit_message>
Rolled my own AStar search
</commit_message>
<xml_diff>
--- a/Game development tracking sheet.xlsx
+++ b/Game development tracking sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul\Documents\S3\asdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D23DA3EA-25DE-4383-89FA-8CCE2C020B9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{48ED45F4-ACC6-401F-9400-BE5B1E590534}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E11" t="s">

</xml_diff>